<commit_message>
added multiple actions for one task
</commit_message>
<xml_diff>
--- a/forms/app/household_member_assessment.xlsx
+++ b/forms/app/household_member_assessment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -333,7 +333,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> experienced symptoms such as diarrhoea or vomiting recently?</t>
+      <t xml:space="preserve"> experienced symptoms such as diarrhea or vomiting recently?</t>
     </r>
   </si>
   <si>
@@ -530,13 +530,13 @@
     <t xml:space="preserve">acute_watery_diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">Acute watery Diarrhea</t>
+    <t xml:space="preserve">Acute watery diarrhea</t>
   </si>
   <si>
     <t xml:space="preserve">profuse_effortless_watery_diarrhoea</t>
   </si>
   <si>
-    <t xml:space="preserve">Profuse effortless watery diarrhoea</t>
+    <t xml:space="preserve">Profuse effortless watery diarrhea</t>
   </si>
   <si>
     <t xml:space="preserve">symptoms</t>
@@ -1144,11 +1144,11 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.49"/>
@@ -4670,10 +4670,10 @@
   <dimension ref="A1:V996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.88"/>
@@ -28692,11 +28692,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.51"/>
@@ -28756,7 +28756,7 @@
       </c>
       <c r="C2" s="49" t="n">
         <f aca="true">NOW()</f>
-        <v>45259.741575122</v>
+        <v>45260.0007077153</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
improved hsehold assessment form
</commit_message>
<xml_diff>
--- a/forms/app/household_member_assessment.xlsx
+++ b/forms/app/household_member_assessment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -902,16 +902,16 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">acute_watery_diarrhea</t>
+    <t xml:space="preserve">acute watery diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">Acute watery Diarrhea</t>
+    <t xml:space="preserve">Acute watery diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">profuse_effortless_watery_diarrhoea</t>
+    <t xml:space="preserve">profuse effortless watery diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">Profuse effortless watery diarrhoea</t>
+    <t xml:space="preserve">Profuse effortless watery diarrhea</t>
   </si>
   <si>
     <t xml:space="preserve">Shock</t>
@@ -1497,11 +1497,11 @@
   </sheetPr>
   <dimension ref="A1:AI1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.49"/>
@@ -3726,9 +3726,7 @@
       <c r="B53" s="19"/>
       <c r="C53" s="10"/>
       <c r="D53" s="20"/>
-      <c r="E53" s="22" t="s">
-        <v>96</v>
-      </c>
+      <c r="E53" s="22"/>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
@@ -5616,11 +5614,11 @@
   </sheetPr>
   <dimension ref="A1:V996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.88"/>
@@ -29643,7 +29641,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.51"/>
@@ -29703,7 +29701,7 @@
       </c>
       <c r="C2" s="51" t="n">
         <f aca="true">NOW()</f>
-        <v>45266.7302626403</v>
+        <v>45317.3570401199</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>191</v>

</xml_diff>